<commit_message>
Finalisation projet et autoprefixer
</commit_message>
<xml_diff>
--- a/Specifications_check.xlsx
+++ b/Specifications_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiengtb/Dropbox/DEVELOPPEMENT/Programmation/01. Développeur Web/Projets OC/Projet 3/damienwill_3_08052021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F33B3D-8352-7045-8C7D-EAE5453DCABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D414AB17-8508-4F44-B9B1-9F2F9C61048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="2980" windowWidth="27240" windowHeight="15060" xr2:uid="{BDE13ED9-C056-E746-98F1-337DCD44526E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="17500" xr2:uid="{BDE13ED9-C056-E746-98F1-337DCD44526E}"/>
   </bookViews>
   <sheets>
     <sheet name="Spécifications" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>Polices</t>
   </si>
@@ -565,6 +565,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,127 +700,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E0C258-0705-0541-8522-5AB2DAB94A7B}">
   <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,101 +1043,101 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="29"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="45"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="48"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="45"/>
-      <c r="B10" s="49" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="56"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
     </row>
     <row r="12" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
       <c r="F12" s="10" t="s">
         <v>32</v>
       </c>
@@ -1149,12 +1149,12 @@
       <c r="A13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
       <c r="F13" s="10" t="s">
         <v>33</v>
       </c>
@@ -1162,12 +1162,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="10" t="s">
         <v>33</v>
       </c>
@@ -1175,12 +1175,12 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="10" t="s">
         <v>33</v>
       </c>
@@ -1188,12 +1188,12 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="10" t="s">
         <v>33</v>
       </c>
@@ -1203,12 +1203,12 @@
       <c r="A17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
       <c r="F17" s="10" t="s">
         <v>33</v>
       </c>
@@ -1216,12 +1216,12 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="10" t="s">
         <v>33</v>
       </c>
@@ -1229,12 +1229,12 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="10" t="s">
         <v>33</v>
       </c>
@@ -1242,38 +1242,40 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="10"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="10"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="60"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="10" t="s">
         <v>33</v>
       </c>
@@ -1283,12 +1285,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="51" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="61"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="10" t="s">
         <v>64</v>
       </c>
@@ -1296,27 +1298,27 @@
     </row>
     <row r="24" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="57" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="45"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="10" t="s">
         <v>33</v>
       </c>
@@ -1389,11 +1391,11 @@
       <c r="B30" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="53" t="s">
+      <c r="C30" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="54"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="10" t="s">
         <v>33</v>
       </c>
@@ -1403,14 +1405,14 @@
     </row>
     <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="58"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="10" t="s">
         <v>33</v>
       </c>
@@ -1420,12 +1422,12 @@
     </row>
     <row r="32" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="52" t="s">
+      <c r="B32" s="31"/>
+      <c r="C32" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="52"/>
-      <c r="E32" s="60"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
       <c r="F32" s="10" t="s">
         <v>33</v>
       </c>
@@ -1437,7 +1439,7 @@
       <c r="A33" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="7"/>
@@ -1450,14 +1452,14 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
-      <c r="B34" s="59"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="25"/>
+      <c r="E34" s="52"/>
       <c r="F34" s="10" t="s">
         <v>33</v>
       </c>
@@ -1467,29 +1469,31 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
-      <c r="B35" s="59"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="10"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G35" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
-      <c r="B36" s="56"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="26"/>
+      <c r="E36" s="64"/>
       <c r="F36" s="10" t="s">
         <v>33</v>
       </c>
@@ -1499,7 +1503,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="8"/>
@@ -1512,7 +1516,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
-      <c r="B38" s="59"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="2" t="s">
         <v>8</v>
       </c>
@@ -1529,7 +1533,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
-      <c r="B39" s="59"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="2" t="s">
         <v>9</v>
       </c>
@@ -1545,8 +1549,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="45"/>
-      <c r="B40" s="56"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="2" t="s">
         <v>10</v>
       </c>
@@ -1565,14 +1569,14 @@
       <c r="A41" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="47"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="34"/>
       <c r="F41" s="10" t="s">
         <v>33</v>
       </c>
@@ -1580,12 +1584,12 @@
     </row>
     <row r="42" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="57" t="s">
+      <c r="B42" s="32"/>
+      <c r="C42" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="57"/>
-      <c r="E42" s="58"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="29"/>
       <c r="F42" s="10" t="s">
         <v>33</v>
       </c>
@@ -1596,26 +1600,26 @@
       <c r="B43" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="53" t="s">
+      <c r="C43" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="53"/>
-      <c r="E43" s="54"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="45"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="53" t="s">
+      <c r="C44" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D44" s="53"/>
-      <c r="E44" s="54"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="10" t="s">
         <v>33</v>
       </c>
@@ -1630,11 +1634,11 @@
       <c r="B45" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="53"/>
-      <c r="E45" s="54"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="10" t="s">
         <v>33</v>
       </c>
@@ -1645,24 +1649,26 @@
       <c r="B46" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="53" t="s">
+      <c r="C46" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D46" s="62"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="10"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="53" t="s">
+      <c r="C47" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="53"/>
-      <c r="E47" s="54"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
       <c r="F47" s="10"/>
       <c r="G47" s="9" t="s">
         <v>72</v>
@@ -1670,12 +1676,12 @@
     </row>
     <row r="48" spans="1:7" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="53" t="s">
+      <c r="B48" s="32"/>
+      <c r="C48" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="53"/>
-      <c r="E48" s="54"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
       <c r="F48" s="10" t="s">
         <v>33</v>
       </c>
@@ -1685,27 +1691,27 @@
     </row>
     <row r="49" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
-      <c r="B49" s="55" t="s">
+      <c r="B49" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="52"/>
-      <c r="E49" s="60"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="28"/>
       <c r="F49" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="45"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="57" t="s">
+      <c r="A50" s="19"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="64"/>
-      <c r="E50" s="65"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="26"/>
       <c r="F50" s="10" t="s">
         <v>33</v>
       </c>
@@ -1713,29 +1719,22 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A22:A32"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="A2:E2"/>
@@ -1752,22 +1751,29 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A22:A32"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Validation W3C html et css - Fin du projet
</commit_message>
<xml_diff>
--- a/Specifications_check.xlsx
+++ b/Specifications_check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiengtb/Dropbox/DEVELOPPEMENT/Programmation/01. Développeur Web/Projets OC/Projet 3/damienwill_3_08052021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D414AB17-8508-4F44-B9B1-9F2F9C61048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EE9DBC-0CB8-5244-AE5D-355E751B8E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27240" windowHeight="17500" xr2:uid="{BDE13ED9-C056-E746-98F1-337DCD44526E}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
   <si>
     <t>Polices</t>
   </si>
   <si>
-    <t>Identité graphique</t>
-  </si>
-  <si>
     <t>Titres</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>L’ensemble du site devra être responsive sur mobile, tablette et desktop.</t>
   </si>
   <si>
-    <t>Les pages devront passer la validation W3C en HTML et CSS sans erreur</t>
-  </si>
-  <si>
     <t>Le site doit être parfaitement compatible avec les dernières versions desktop de Chrome et Firefox.</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
   </si>
   <si>
     <t>Header</t>
-  </si>
-  <si>
-    <t>Composition</t>
   </si>
   <si>
     <t>Affichage de la localisation des restaurants. À terme il sera possible de choisir sa localisation pour trouver des restaurants proches d’un certain lieu.</t>
@@ -255,6 +246,18 @@
   </si>
   <si>
     <t>Video</t>
+  </si>
+  <si>
+    <t>Composition HTML</t>
+  </si>
+  <si>
+    <t>Identité graphique et design CSS</t>
+  </si>
+  <si>
+    <t>Les pages devront passer la validation W3C en HTML sans erreur</t>
+  </si>
+  <si>
+    <t>Les pages devront passer la validation W3C en CSS sans erreur</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,16 +520,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -565,9 +562,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -704,6 +713,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1027,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E0C258-0705-0541-8522-5AB2DAB94A7B}">
-  <dimension ref="A2:G50"/>
+  <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,709 +1065,767 @@
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="97.33203125" customWidth="1"/>
     <col min="5" max="5" width="32.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="31.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="31.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="2" spans="1:8" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="35" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="B6" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="48"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="B9" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="55" t="s">
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="63"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="65"/>
+    </row>
+    <row r="12" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="56"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="61"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
-    </row>
-    <row r="12" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="C20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="59"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="27" t="s">
+      <c r="D22" s="26"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="20"/>
+      <c r="B28" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="17" t="s">
+      <c r="D29" s="26"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="20"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="20"/>
+      <c r="B31" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="19"/>
-    </row>
-    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16" t="s">
+      <c r="B32" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="31"/>
+      <c r="D33" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="54"/>
+      <c r="F33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="31"/>
+      <c r="D34" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="54"/>
+      <c r="F34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="16"/>
+      <c r="H34" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="52"/>
-      <c r="F35" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="64" t="s">
+      <c r="E35" s="66"/>
+      <c r="F35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="20"/>
+      <c r="B36" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="64"/>
-      <c r="F36" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="30" t="s">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="20"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="20"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="2" t="s">
+      <c r="F38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="20"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="30" t="s">
+      <c r="E39" s="73"/>
+      <c r="F39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="20"/>
+      <c r="B40" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="B41" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="H41" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="20"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="42" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G42" s="9"/>
-    </row>
-    <row r="43" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="12" t="s">
+      <c r="D43" s="26"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="20" t="s">
+      <c r="D44" s="22"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+      <c r="B45" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>53</v>
-      </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G45" s="9"/>
-    </row>
-    <row r="46" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="23"/>
-      <c r="F46" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" ht="86" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="132" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="27" t="s">
+      <c r="F46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="24"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="27"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="19"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="25"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G50" s="11"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="21"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="27"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="18"/>
+      <c r="H51" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="A17:A21"/>
+  <mergeCells count="56">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A11:E11"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="B6:E8"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A32:A41"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
@@ -1751,29 +1836,29 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="B48:B49"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A20:A31"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A22:A32"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C51:E51"/>
     <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>